<commit_message>
Various Changes to Design docs
- Card costs updated
- Creature Stats rebalanced
- various docs moved to Archive
</commit_message>
<xml_diff>
--- a/Game Design/Cards.xlsx
+++ b/Game Design/Cards.xlsx
@@ -548,7 +548,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H3" s="2">
         <v>2</v>
@@ -668,10 +668,10 @@
         <v>11</v>
       </c>
       <c r="G4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
@@ -696,7 +696,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5" s="2">
         <v>4</v>
@@ -752,10 +752,10 @@
         <v>14</v>
       </c>
       <c r="G7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>

</xml_diff>